<commit_message>
commit alteracao dados solo
</commit_message>
<xml_diff>
--- a/dados/solos.xlsx
+++ b/dados/solos.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +631,7 @@
         <v>15.42</v>
       </c>
       <c r="E2" s="5">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5009999999999998E-2</v>
       </c>
       <c r="F2" s="5">
         <v>0.63500000000000001</v>
@@ -681,7 +681,7 @@
         <v>17.484999999999999</v>
       </c>
       <c r="E3" s="5">
-        <v>0.09</v>
+        <v>9.01E-2</v>
       </c>
       <c r="F3" s="5">
         <v>0.32</v>
@@ -1779,7 +1779,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
enviando alteração análise de solos
</commit_message>
<xml_diff>
--- a/dados/solos.xlsx
+++ b/dados/solos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CL2022\BancoDadosAgroflorestal\App2\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7EAF5B-EC12-47A5-BC1D-9AD01A6E4B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analise" sheetId="1" r:id="rId1"/>
@@ -175,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,15 +271,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,16 +557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -607,54 +606,54 @@
       <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>3.9</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <v>10.8</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>15.42</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>6.5009999999999998E-2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <v>0.63500000000000001</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2">
         <v>0.315</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2">
         <v>3.3650000000000002</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2">
         <v>0.94</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2">
         <v>0.35</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2">
         <v>161</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2">
         <v>1.7000000000000002</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>1.95</v>
       </c>
       <c r="N2">
@@ -667,44 +666,44 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3">
         <v>3.75</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>17.484999999999999</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3">
         <v>9.01E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>0.32</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3">
         <v>0.26500000000000001</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>2.145</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3">
         <v>1.03</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3">
         <v>0.65</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3">
         <v>42</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3">
         <v>1.7</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3">
         <v>12.299999999999999</v>
       </c>
       <c r="N3">
@@ -717,44 +716,44 @@
         <v>67.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>4.05</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>1.05</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>8.9849999999999994</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>0.08</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>0.91500000000000004</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>0.4</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>2.2350000000000003</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4">
         <v>0.61</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4">
         <v>0.60000000000000009</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4">
         <v>4</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4">
         <v>1.4500000000000002</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4">
         <v>32.950000000000003</v>
       </c>
       <c r="N4">
@@ -767,44 +766,44 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>4.55</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>4.3499999999999996</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>16.045000000000002</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>1.4850000000000001</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>1.0350000000000001</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>3.25</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5">
         <v>0.51</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5">
         <v>0.1</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5">
         <v>113.5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5">
         <v>0.8</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5">
         <v>1.1000000000000001</v>
       </c>
       <c r="N5">
@@ -817,44 +816,44 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>4.45</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <v>4.5</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>18.5</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>7.5000000000000011E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>1.8250000000000002</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>0.95499999999999996</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <v>1.9700000000000002</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6">
         <v>0.33</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6">
         <v>2.8</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6">
         <v>21.5</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6">
         <v>0.79999999999999993</v>
       </c>
       <c r="N6">
@@ -867,44 +866,44 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>4.75</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <v>7.95</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>8.4999999999999992E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>1.2450000000000001</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <v>1.9350000000000001</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7">
         <v>0.36</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7">
         <v>3.4</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7">
         <v>33</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7">
         <v>3.9</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7">
         <v>2.8499999999999996</v>
       </c>
       <c r="N7">
@@ -917,44 +916,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>4.2</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8">
         <v>0.44999999999999996</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>19.855</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8">
         <v>1.345</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8">
         <v>0.86</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <v>2.3049999999999997</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8">
         <v>0.90999999999999992</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8">
         <v>3.15</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8">
         <v>23</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8">
         <v>4.5</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8">
         <v>1.2999999999999998</v>
       </c>
       <c r="N8">
@@ -967,44 +966,44 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <v>1.6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>4.2050000000000001</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9">
         <v>0.84</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9">
         <v>0.62</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <v>2.2549999999999999</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9">
         <v>0.41000000000000003</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9">
         <v>20.5</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9">
         <v>2.5999999999999996</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9">
         <v>0.9</v>
       </c>
       <c r="N9">
@@ -1017,44 +1016,44 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>4.3</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10">
         <v>0.9</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>14.66</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10">
         <v>1.4850000000000001</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>0.53</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <v>2.57</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10">
         <v>0.62</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10">
         <v>28</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10">
         <v>4.05</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10">
         <v>1.45</v>
       </c>
       <c r="N10">
@@ -1067,44 +1066,44 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11">
         <v>5.5000000000000007E-2</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11">
         <v>0.89</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <v>0.39500000000000002</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11">
         <v>2.38</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11">
         <v>0.38</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11">
         <v>0.30000000000000004</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11">
         <v>110</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11">
         <v>1.65</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11">
         <v>1.25</v>
       </c>
       <c r="N11">
@@ -1117,44 +1116,44 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>14.1</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12">
         <v>6.9749999999999996</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12">
         <v>1.875</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <v>0.66500000000000004</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <v>3.0250000000000004</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12">
         <v>0.57000000000000006</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12">
         <v>0.15000000000000002</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12">
         <v>120</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12">
         <v>1.4500000000000002</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12">
         <v>1.85</v>
       </c>
       <c r="N12">
@@ -1167,44 +1166,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>4.2</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13">
         <v>3.3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>14.845000000000001</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13">
         <v>0.47000000000000003</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13">
         <v>4.1449999999999996</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13">
         <v>0.42</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13">
         <v>0.15000000000000002</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13">
         <v>131.5</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13">
         <v>1.4</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
         <v>1.9</v>
       </c>
       <c r="N13">
@@ -1217,44 +1216,44 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>4.1999999999999993</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>7.03</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>0.08</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14">
         <v>1.395</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14">
         <v>0.45</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <v>3.2199999999999998</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14">
         <v>0.41000000000000003</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14">
         <v>0.1</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14">
         <v>137</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14">
         <v>3.05</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14">
         <v>2.1</v>
       </c>
       <c r="N14">
@@ -1267,44 +1266,44 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15">
         <v>4.25</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
         <v>1.2000000000000002</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15">
         <v>10.065</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15">
         <v>0.1</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15">
         <v>1.33</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15">
         <v>0.35</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15">
         <v>2.12</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15">
         <v>0.65</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15">
         <v>2.25</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15">
         <v>30</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15">
         <v>1.9</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15">
         <v>0.85000000000000009</v>
       </c>
       <c r="N15">
@@ -1317,44 +1316,44 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16">
         <v>4.3</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16">
         <v>5.6999999999999993</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <v>8.5499999999999989</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16">
         <v>0.10500000000000001</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16">
         <v>1.845</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16">
         <v>0.45499999999999996</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16">
         <v>3.0449999999999999</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16">
         <v>0.43</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16">
         <v>0.30000000000000004</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16">
         <v>129</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16">
         <v>1.5</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16">
         <v>1.7</v>
       </c>
       <c r="N16">
@@ -1367,44 +1366,44 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>4.1500000000000004</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17">
         <v>12.819999999999999</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>0.11</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17">
         <v>1.3699999999999999</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17">
         <v>0.37</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17">
         <v>1.9750000000000001</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17">
         <v>0.71</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17">
         <v>2.9000000000000004</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17">
         <v>25.5</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17">
         <v>2.4000000000000004</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17">
         <v>0.75</v>
       </c>
       <c r="N17">
@@ -1416,46 +1415,46 @@
       <c r="P17">
         <v>13</v>
       </c>
-      <c r="U17" s="8"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18">
         <v>0.25</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18">
         <v>9.495000000000001</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18">
         <v>0.85</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18">
         <v>0.315</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18">
         <v>1.9450000000000001</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18">
         <v>0.44999999999999996</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18">
         <v>3.5999999999999996</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18">
         <v>35</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18">
         <v>4.2</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18">
         <v>1.65</v>
       </c>
       <c r="N18">
@@ -1468,44 +1467,44 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19">
         <v>1.55</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19">
         <v>6.5500000000000007</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19">
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19">
         <v>0.6</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19">
         <v>0.245</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19">
         <v>2.7050000000000001</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19">
         <v>0.31</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19">
         <v>0.9</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19">
         <v>39</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19">
         <v>13.3</v>
       </c>
       <c r="N19">
@@ -1518,44 +1517,44 @@
         <v>47.7</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20">
         <v>4.3</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20">
         <v>0.45</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20">
         <v>18.945</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20">
         <v>0.95000000000000007</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20">
         <v>0.54500000000000004</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20">
         <v>2.23</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20">
         <v>0.53</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20">
         <v>2.25</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20">
         <v>15.5</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20">
         <v>2.1</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20">
         <v>1.4</v>
       </c>
       <c r="N20">
@@ -1568,44 +1567,44 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21">
         <v>0.15000000000000002</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21">
         <v>8.754999999999999</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21">
         <v>1.58</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21">
         <v>0.75</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21">
         <v>2.0550000000000002</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21">
         <v>0.41000000000000003</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21">
         <v>2.95</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21">
         <v>24</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21">
         <v>3.4000000000000004</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21">
         <v>1.5999999999999999</v>
       </c>
       <c r="N21">
@@ -1618,44 +1617,44 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>4.5</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22">
         <v>2.75</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22">
         <v>18.37</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22">
         <v>5.5E-2</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22">
         <v>1.67</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22">
         <v>0.94</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22">
         <v>3.22</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22">
         <v>0.36</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22">
         <v>0.15000000000000002</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22">
         <v>102.5</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22">
         <v>3.5</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22">
         <v>1</v>
       </c>
       <c r="N22">
@@ -1668,44 +1667,44 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23">
         <v>4.3499999999999996</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23">
         <v>3.4499999999999997</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23">
         <v>11.41</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23">
         <v>1.2749999999999999</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23">
         <v>0.94</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23">
         <v>2.5949999999999998</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23">
         <v>0.46</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23">
         <v>0.15000000000000002</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23">
         <v>95.5</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23">
         <v>1.25</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23">
         <v>1.2</v>
       </c>
       <c r="N23">
@@ -1718,44 +1717,44 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24">
         <v>1.9</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24">
         <v>1.5</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24">
         <v>0.57000000000000006</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24">
         <v>2.0449999999999999</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24">
         <v>0.31</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24">
         <v>3.45</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24">
         <v>34.5</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24">
         <v>2.9000000000000004</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24">
         <v>1.95</v>
       </c>
       <c r="N24">
@@ -1775,16 +1774,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1824,17 +1823,17 @@
       <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1884,10 +1883,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1908,14 +1907,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1935,11 +1934,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>1.57</v>
       </c>
       <c r="C2">
@@ -1955,11 +1954,11 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>0.44</v>
       </c>
       <c r="C3">
@@ -1975,11 +1974,11 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.64</v>
       </c>
       <c r="C4">
@@ -1995,7 +1994,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2015,7 +2014,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -2115,7 +2114,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -2175,7 +2174,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>

</xml_diff>